<commit_message>
Update: QA Excel Compiler - STATUS tracking
- Added STATUS column compilation (STATUS_{Username})
- Valid STATUS values: ISSUE, NO ISSUE, BLOCKED
- Completion % now based on STATUS (not COMMENT)
- Updated mock test files with valid STATUS values

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/miniprojects/qa_excel_compiler/Masterfolder/Master_Quest.xlsx
+++ b/miniprojects/qa_excel_compiler/Masterfolder/Master_Quest.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,25 +451,40 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>STATUS_John</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>STATUS_Bob</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>STATUS_Alice</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>COMMENT_John</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>COMMENT_Bob</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>COMMENT_Alice</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
           <t>COMMENT</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>COMMENT_John</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>COMMENT_Bob</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>COMMENT_Alice</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>SCREENSHOT</t>
         </is>
@@ -489,10 +504,19 @@
       <c r="C2" t="n">
         <v>10001</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>"Actually found another issue here" (date: 251230 1213)
-"Translation looks good" (date: 251230 1213)</t>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>NO ISSUE</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NO ISSUE</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>"Translation looks good" (date: 251230 1219)</t>
         </is>
       </c>
     </row>
@@ -510,19 +534,34 @@
       <c r="C3" t="n">
         <v>1000157</v>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>ISSUE</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>"Typo: should be 'Strange Land' singular" (date: 251230 1213)</t>
+          <t>ISSUE</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>"Agree with John - typo" (date: 251230 1213)</t>
+          <t>NO ISSUE</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>"I think it's fine actually" (date: 251230 1213)</t>
+          <t>"Typo: should be singular" (date: 251230 1219)</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>"Agree - typo" (date: 251230 1219)</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>"I think it's fine" (date: 251230 1219)</t>
         </is>
       </c>
     </row>
@@ -540,9 +579,14 @@
       <c r="C4" t="n">
         <v>1000200</v>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>"Missing article 'the'" (date: 251230 1213)</t>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>ISSUE</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>"Missing article" (date: 251230 1219)</t>
         </is>
       </c>
     </row>
@@ -560,14 +604,24 @@
       <c r="C5" t="n">
         <v>1000201</v>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>NO ISSUE</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>"Perfect" (date: 251230 1213)</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>"Good translation" (date: 251230 1213)</t>
+          <t>NO ISSUE</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>"Perfect" (date: 251230 1219)</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>"Good" (date: 251230 1219)</t>
         </is>
       </c>
     </row>
@@ -585,9 +639,14 @@
       <c r="C6" t="n">
         <v>1000202</v>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>"Forest should be woods" (date: 251230 1213)</t>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>ISSUE</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>"Forest should be woods" (date: 251230 1219)</t>
         </is>
       </c>
     </row>
@@ -602,7 +661,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -638,25 +697,40 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>STATUS_John</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>STATUS_Bob</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>STATUS_Alice</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>COMMENT_John</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>COMMENT_Bob</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>COMMENT_Alice</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
           <t>COMMENT</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>COMMENT_John</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>COMMENT_Bob</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>COMMENT_Alice</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>SCREENSHOT</t>
         </is>
@@ -676,14 +750,24 @@
       <c r="C2" t="n">
         <v>2000001</v>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>NO ISSUE</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>"Verified" (date: 251230 1213)</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>"All good" (date: 251230 1213)</t>
+          <t>NO ISSUE</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>"Verified" (date: 251230 1219)</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>"All good" (date: 251230 1219)</t>
         </is>
       </c>
     </row>
@@ -701,14 +785,24 @@
       <c r="C3" t="n">
         <v>2000002</v>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NO ISSUE</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>"Verified shop text" (date: 251230 1213)</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>"Shop translation verified" (date: 251230 1213)</t>
+          <t>NO ISSUE</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>"Verified" (date: 251230 1219)</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>"Shop verified" (date: 251230 1219)</t>
         </is>
       </c>
     </row>
@@ -726,14 +820,24 @@
       <c r="C4" t="n">
         <v>2000003</v>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>BLOCKED</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>"Need to check context" (date: 251230 1213)</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>"Quest complete is correct" (date: 251230 1213)</t>
+          <t>NO ISSUE</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>"Need to check context" (date: 251230 1219)</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>"Correct" (date: 251230 1219)</t>
         </is>
       </c>
     </row>
@@ -786,7 +890,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>40.0%</t>
+          <t>60.0%</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -796,7 +900,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>36.6%</t>
+          <t>46.6%</t>
         </is>
       </c>
     </row>

</xml_diff>